<commit_message>
rettet tekst feil i invariant
</commit_message>
<xml_diff>
--- a/StructureDefinition-hn-basis-appointment.xlsx
+++ b/StructureDefinition-hn-basis-appointment.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4591" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4591" uniqueCount="621">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-01-31T12:01:35+01:00</t>
+    <t>2025-01-31T15:15:59+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1552,7 +1552,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-must-be-max-100-chars:Length MUST be &lt;=1000. {$this.length() &lt;= 1000}</t>
+must-be-max-1000-chars:Length MUST be &lt;= 1000 {$this.length() &lt;= 1000}</t>
   </si>
   <si>
     <t>.text</t>
@@ -1726,10 +1726,6 @@
   </si>
   <si>
     <t>While Appointment.comment contains information for internal use, Appointment.patientInstructions is used to capture patient facing information about the Appointment (e.g. please bring your referral or fast from 8pm night before).</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-must-be-max-500-chars:Length MUST be &lt;= 1000 {$this.length() &lt;= 1000}</t>
   </si>
   <si>
     <t>DESCRIPTION (for patient use)</t>
@@ -14946,7 +14942,7 @@
         <v>100</v>
       </c>
       <c r="AJ108" t="s" s="2">
-        <v>551</v>
+        <v>494</v>
       </c>
       <c r="AK108" t="s" s="2">
         <v>20</v>
@@ -14955,7 +14951,7 @@
         <v>546</v>
       </c>
       <c r="AM108" t="s" s="2">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="AN108" t="s" s="2">
         <v>20</v>
@@ -14966,14 +14962,14 @@
     </row>
     <row r="109" hidden="true">
       <c r="A109" t="s" s="2">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B109" t="s" s="2">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C109" s="2"/>
       <c r="D109" t="s" s="2">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E109" s="2"/>
       <c r="F109" t="s" s="2">
@@ -14992,13 +14988,13 @@
         <v>20</v>
       </c>
       <c r="K109" t="s" s="2">
+        <v>554</v>
+      </c>
+      <c r="L109" t="s" s="2">
         <v>555</v>
       </c>
-      <c r="L109" t="s" s="2">
+      <c r="M109" t="s" s="2">
         <v>556</v>
-      </c>
-      <c r="M109" t="s" s="2">
-        <v>557</v>
       </c>
       <c r="N109" t="s" s="2">
         <v>478</v>
@@ -15051,7 +15047,7 @@
         <v>20</v>
       </c>
       <c r="AF109" t="s" s="2">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="AG109" t="s" s="2">
         <v>78</v>
@@ -15066,10 +15062,10 @@
         <v>358</v>
       </c>
       <c r="AK109" t="s" s="2">
+        <v>557</v>
+      </c>
+      <c r="AL109" t="s" s="2">
         <v>558</v>
-      </c>
-      <c r="AL109" t="s" s="2">
-        <v>559</v>
       </c>
       <c r="AM109" t="s" s="2">
         <v>20</v>
@@ -15083,10 +15079,10 @@
     </row>
     <row r="110" hidden="true">
       <c r="A110" t="s" s="2">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B110" t="s" s="2">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C110" s="2"/>
       <c r="D110" t="s" s="2">
@@ -15109,13 +15105,13 @@
         <v>20</v>
       </c>
       <c r="K110" t="s" s="2">
+        <v>560</v>
+      </c>
+      <c r="L110" t="s" s="2">
         <v>561</v>
       </c>
-      <c r="L110" t="s" s="2">
+      <c r="M110" t="s" s="2">
         <v>562</v>
-      </c>
-      <c r="M110" t="s" s="2">
-        <v>563</v>
       </c>
       <c r="N110" s="2"/>
       <c r="O110" s="2"/>
@@ -15166,7 +15162,7 @@
         <v>20</v>
       </c>
       <c r="AF110" t="s" s="2">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="AG110" t="s" s="2">
         <v>88</v>
@@ -15178,30 +15174,30 @@
         <v>100</v>
       </c>
       <c r="AJ110" t="s" s="2">
+        <v>563</v>
+      </c>
+      <c r="AK110" t="s" s="2">
         <v>564</v>
       </c>
-      <c r="AK110" t="s" s="2">
+      <c r="AL110" t="s" s="2">
         <v>565</v>
       </c>
-      <c r="AL110" t="s" s="2">
+      <c r="AM110" t="s" s="2">
         <v>566</v>
       </c>
-      <c r="AM110" t="s" s="2">
+      <c r="AN110" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AO110" t="s" s="2">
         <v>567</v>
-      </c>
-      <c r="AN110" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AO110" t="s" s="2">
-        <v>568</v>
       </c>
     </row>
     <row r="111" hidden="true">
       <c r="A111" t="s" s="2">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B111" t="s" s="2">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C111" s="2"/>
       <c r="D111" t="s" s="2">
@@ -15313,10 +15309,10 @@
     </row>
     <row r="112" hidden="true">
       <c r="A112" t="s" s="2">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B112" t="s" s="2">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C112" s="2"/>
       <c r="D112" t="s" s="2">
@@ -15430,14 +15426,14 @@
     </row>
     <row r="113" hidden="true">
       <c r="A113" t="s" s="2">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B113" t="s" s="2">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C113" s="2"/>
       <c r="D113" t="s" s="2">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E113" s="2"/>
       <c r="F113" t="s" s="2">
@@ -15459,10 +15455,10 @@
         <v>111</v>
       </c>
       <c r="L113" t="s" s="2">
+        <v>572</v>
+      </c>
+      <c r="M113" t="s" s="2">
         <v>573</v>
-      </c>
-      <c r="M113" t="s" s="2">
-        <v>574</v>
       </c>
       <c r="N113" t="s" s="2">
         <v>114</v>
@@ -15517,7 +15513,7 @@
         <v>20</v>
       </c>
       <c r="AF113" t="s" s="2">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="AG113" t="s" s="2">
         <v>78</v>
@@ -15549,10 +15545,10 @@
     </row>
     <row r="114" hidden="true">
       <c r="A114" t="s" s="2">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B114" t="s" s="2">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C114" s="2"/>
       <c r="D114" t="s" s="2">
@@ -15578,13 +15574,13 @@
         <v>317</v>
       </c>
       <c r="L114" t="s" s="2">
+        <v>576</v>
+      </c>
+      <c r="M114" t="s" s="2">
         <v>577</v>
       </c>
-      <c r="M114" t="s" s="2">
+      <c r="N114" t="s" s="2">
         <v>578</v>
-      </c>
-      <c r="N114" t="s" s="2">
-        <v>579</v>
       </c>
       <c r="O114" s="2"/>
       <c r="P114" t="s" s="2">
@@ -15613,11 +15609,11 @@
         <v>148</v>
       </c>
       <c r="Y114" t="s" s="2">
+        <v>579</v>
+      </c>
+      <c r="Z114" t="s" s="2">
         <v>580</v>
       </c>
-      <c r="Z114" t="s" s="2">
-        <v>581</v>
-      </c>
       <c r="AA114" t="s" s="2">
         <v>20</v>
       </c>
@@ -15634,7 +15630,7 @@
         <v>20</v>
       </c>
       <c r="AF114" t="s" s="2">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="AG114" t="s" s="2">
         <v>78</v>
@@ -15652,7 +15648,7 @@
         <v>20</v>
       </c>
       <c r="AL114" t="s" s="2">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AM114" t="s" s="2">
         <v>108</v>
@@ -15661,15 +15657,15 @@
         <v>20</v>
       </c>
       <c r="AO114" t="s" s="2">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="115" hidden="true">
       <c r="A115" t="s" s="2">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B115" t="s" s="2">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C115" s="2"/>
       <c r="D115" t="s" s="2">
@@ -15781,10 +15777,10 @@
     </row>
     <row r="116" hidden="true">
       <c r="A116" t="s" s="2">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B116" t="s" s="2">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C116" s="2"/>
       <c r="D116" t="s" s="2">
@@ -15898,10 +15894,10 @@
     </row>
     <row r="117" hidden="true">
       <c r="A117" t="s" s="2">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B117" t="s" s="2">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C117" s="2"/>
       <c r="D117" t="s" s="2">
@@ -16017,10 +16013,10 @@
     </row>
     <row r="118" hidden="true">
       <c r="A118" t="s" s="2">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B118" t="s" s="2">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C118" s="2"/>
       <c r="D118" t="s" s="2">
@@ -16136,10 +16132,10 @@
     </row>
     <row r="119" hidden="true">
       <c r="A119" t="s" s="2">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B119" t="s" s="2">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C119" s="2"/>
       <c r="D119" t="s" s="2">
@@ -16162,13 +16158,13 @@
         <v>89</v>
       </c>
       <c r="K119" t="s" s="2">
+        <v>588</v>
+      </c>
+      <c r="L119" t="s" s="2">
         <v>589</v>
       </c>
-      <c r="L119" t="s" s="2">
+      <c r="M119" t="s" s="2">
         <v>590</v>
-      </c>
-      <c r="M119" t="s" s="2">
-        <v>591</v>
       </c>
       <c r="N119" t="s" s="2">
         <v>478</v>
@@ -16221,7 +16217,7 @@
         <v>20</v>
       </c>
       <c r="AF119" t="s" s="2">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="AG119" t="s" s="2">
         <v>78</v>
@@ -16239,24 +16235,24 @@
         <v>20</v>
       </c>
       <c r="AL119" t="s" s="2">
+        <v>591</v>
+      </c>
+      <c r="AM119" t="s" s="2">
         <v>592</v>
       </c>
-      <c r="AM119" t="s" s="2">
+      <c r="AN119" t="s" s="2">
         <v>593</v>
       </c>
-      <c r="AN119" t="s" s="2">
+      <c r="AO119" t="s" s="2">
         <v>594</v>
-      </c>
-      <c r="AO119" t="s" s="2">
-        <v>595</v>
       </c>
     </row>
     <row r="120" hidden="true">
       <c r="A120" t="s" s="2">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B120" t="s" s="2">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C120" s="2"/>
       <c r="D120" t="s" s="2">
@@ -16282,10 +16278,10 @@
         <v>168</v>
       </c>
       <c r="L120" t="s" s="2">
+        <v>596</v>
+      </c>
+      <c r="M120" t="s" s="2">
         <v>597</v>
-      </c>
-      <c r="M120" t="s" s="2">
-        <v>598</v>
       </c>
       <c r="N120" t="s" s="2">
         <v>493</v>
@@ -16317,11 +16313,11 @@
         <v>221</v>
       </c>
       <c r="Y120" t="s" s="2">
+        <v>598</v>
+      </c>
+      <c r="Z120" t="s" s="2">
         <v>599</v>
       </c>
-      <c r="Z120" t="s" s="2">
-        <v>600</v>
-      </c>
       <c r="AA120" t="s" s="2">
         <v>20</v>
       </c>
@@ -16338,7 +16334,7 @@
         <v>20</v>
       </c>
       <c r="AF120" t="s" s="2">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="AG120" t="s" s="2">
         <v>78</v>
@@ -16356,10 +16352,10 @@
         <v>20</v>
       </c>
       <c r="AL120" t="s" s="2">
+        <v>600</v>
+      </c>
+      <c r="AM120" t="s" s="2">
         <v>601</v>
-      </c>
-      <c r="AM120" t="s" s="2">
-        <v>602</v>
       </c>
       <c r="AN120" t="s" s="2">
         <v>20</v>
@@ -16370,10 +16366,10 @@
     </row>
     <row r="121" hidden="true">
       <c r="A121" t="s" s="2">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B121" t="s" s="2">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C121" s="2"/>
       <c r="D121" t="s" s="2">
@@ -16399,10 +16395,10 @@
         <v>168</v>
       </c>
       <c r="L121" t="s" s="2">
+        <v>603</v>
+      </c>
+      <c r="M121" t="s" s="2">
         <v>604</v>
-      </c>
-      <c r="M121" t="s" s="2">
-        <v>605</v>
       </c>
       <c r="N121" t="s" s="2">
         <v>493</v>
@@ -16434,11 +16430,11 @@
         <v>221</v>
       </c>
       <c r="Y121" t="s" s="2">
+        <v>605</v>
+      </c>
+      <c r="Z121" t="s" s="2">
         <v>606</v>
       </c>
-      <c r="Z121" t="s" s="2">
-        <v>607</v>
-      </c>
       <c r="AA121" t="s" s="2">
         <v>20</v>
       </c>
@@ -16455,7 +16451,7 @@
         <v>20</v>
       </c>
       <c r="AF121" t="s" s="2">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="AG121" t="s" s="2">
         <v>88</v>
@@ -16473,24 +16469,24 @@
         <v>20</v>
       </c>
       <c r="AL121" t="s" s="2">
+        <v>607</v>
+      </c>
+      <c r="AM121" t="s" s="2">
         <v>608</v>
       </c>
-      <c r="AM121" t="s" s="2">
+      <c r="AN121" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AO121" t="s" s="2">
         <v>609</v>
-      </c>
-      <c r="AN121" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AO121" t="s" s="2">
-        <v>610</v>
       </c>
     </row>
     <row r="122" hidden="true">
       <c r="A122" t="s" s="2">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B122" t="s" s="2">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C122" s="2"/>
       <c r="D122" t="s" s="2">
@@ -16516,10 +16512,10 @@
         <v>344</v>
       </c>
       <c r="L122" t="s" s="2">
+        <v>611</v>
+      </c>
+      <c r="M122" t="s" s="2">
         <v>612</v>
-      </c>
-      <c r="M122" t="s" s="2">
-        <v>613</v>
       </c>
       <c r="N122" t="s" s="2">
         <v>347</v>
@@ -16572,7 +16568,7 @@
         <v>20</v>
       </c>
       <c r="AF122" t="s" s="2">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="AG122" t="s" s="2">
         <v>78</v>
@@ -16590,24 +16586,24 @@
         <v>20</v>
       </c>
       <c r="AL122" t="s" s="2">
+        <v>613</v>
+      </c>
+      <c r="AM122" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AN122" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AO122" t="s" s="2">
         <v>614</v>
-      </c>
-      <c r="AM122" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AN122" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AO122" t="s" s="2">
-        <v>615</v>
       </c>
     </row>
     <row r="123" hidden="true">
       <c r="A123" t="s" s="2">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B123" t="s" s="2">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C123" s="2"/>
       <c r="D123" t="s" s="2">
@@ -16633,13 +16629,13 @@
         <v>344</v>
       </c>
       <c r="L123" t="s" s="2">
+        <v>616</v>
+      </c>
+      <c r="M123" t="s" s="2">
         <v>617</v>
       </c>
-      <c r="M123" t="s" s="2">
+      <c r="N123" t="s" s="2">
         <v>618</v>
-      </c>
-      <c r="N123" t="s" s="2">
-        <v>619</v>
       </c>
       <c r="O123" s="2"/>
       <c r="P123" t="s" s="2">
@@ -16689,7 +16685,7 @@
         <v>20</v>
       </c>
       <c r="AF123" t="s" s="2">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="AG123" t="s" s="2">
         <v>78</v>
@@ -16707,16 +16703,16 @@
         <v>510</v>
       </c>
       <c r="AL123" t="s" s="2">
+        <v>619</v>
+      </c>
+      <c r="AM123" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AN123" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AO123" t="s" s="2">
         <v>620</v>
-      </c>
-      <c r="AM123" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AN123" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AO123" t="s" s="2">
-        <v>621</v>
       </c>
     </row>
   </sheetData>

</xml_diff>